<commit_message>
Fixed up button and main menu
</commit_message>
<xml_diff>
--- a/TaskPlan.xlsx
+++ b/TaskPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Martin\Documents\Programing teaching\PuzzleGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153FADE7-9803-493F-8CC5-60C2550ACF17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3537B9-FF14-4E97-965E-306121E2E346}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="495" yWindow="120" windowWidth="25530" windowHeight="13470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
   <si>
     <t>Detailed task</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>In progress</t>
+  </si>
+  <si>
+    <t>Fix font problem</t>
   </si>
 </sst>
 </file>
@@ -228,14 +231,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -526,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,12 +754,17 @@
         <v>47</v>
       </c>
     </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="In progress">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="In progress">
       <formula>NOT(ISERROR(SEARCH("In progress",D1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>